<commit_message>
add: test-Tree todo: pattern for generation users and books, add book-list for users, add Tree with books and users
</commit_message>
<xml_diff>
--- a/src/main/resources/com/example/lab5/books.xlsx
+++ b/src/main/resources/com/example/lab5/books.xlsx
@@ -8,12 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\lab5\src\main\resources\com\example\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6308D23-35D4-4704-A43D-14116684108D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA9B8D6-95E8-43D4-909B-24E831ED6FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17436" yWindow="948" windowWidth="11112" windowHeight="9684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10032" yWindow="1560" windowWidth="11112" windowHeight="9684" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ру_уч" sheetId="1" r:id="rId1"/>
+    <sheet name="en_уч" sheetId="2" r:id="rId2"/>
+    <sheet name="en_un" sheetId="3" r:id="rId3"/>
+    <sheet name="en_au" sheetId="4" r:id="rId4"/>
+    <sheet name="ру_фик" sheetId="5" r:id="rId5"/>
+    <sheet name="ру_авт" sheetId="6" r:id="rId6"/>
+    <sheet name="en_fic" sheetId="7" r:id="rId7"/>
+    <sheet name="en_fic_au" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>Реакторное материаловедение</t>
   </si>
@@ -85,6 +92,363 @@
   </si>
   <si>
     <t>Ядерное топливо</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>Deep learning</t>
+  </si>
+  <si>
+    <t>IBM Data Science</t>
+  </si>
+  <si>
+    <t>Neural Networks</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Spatial Analysis</t>
+  </si>
+  <si>
+    <t>Sattellite Imagery</t>
+  </si>
+  <si>
+    <t>Data Warehouse</t>
+  </si>
+  <si>
+    <t>Marketing Analytics</t>
+  </si>
+  <si>
+    <t>Vital Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DevOps </t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>AI Product Management</t>
+  </si>
+  <si>
+    <t>Johns Hopkins University</t>
+  </si>
+  <si>
+    <t>Duke University</t>
+  </si>
+  <si>
+    <t>University of Colorado Boulder</t>
+  </si>
+  <si>
+    <t>Imperial College London</t>
+  </si>
+  <si>
+    <t>University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Macquarie University</t>
+  </si>
+  <si>
+    <t>University of California San Diego</t>
+  </si>
+  <si>
+    <t>Eindhoven University of Technology</t>
+  </si>
+  <si>
+    <t>Rice University</t>
+  </si>
+  <si>
+    <t>University of Zurich</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>Stanford University</t>
+  </si>
+  <si>
+    <t>CFA Institute</t>
+  </si>
+  <si>
+    <t>Princeton University</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>Jon Reifschneider  </t>
+  </si>
+  <si>
+    <t>Timothy C. Urdan</t>
+  </si>
+  <si>
+    <t>Allen B. Downey.</t>
+  </si>
+  <si>
+    <t>Daniela Witten</t>
+  </si>
+  <si>
+    <t>Trevor Hastie</t>
+  </si>
+  <si>
+    <t>Robert Tibshirani</t>
+  </si>
+  <si>
+    <t>Gareth James</t>
+  </si>
+  <si>
+    <t>David Morin</t>
+  </si>
+  <si>
+    <t>William Feller</t>
+  </si>
+  <si>
+    <t>Andriy Burkov</t>
+  </si>
+  <si>
+    <t>Andreas C. Müller</t>
+  </si>
+  <si>
+    <t>Sarah Guido</t>
+  </si>
+  <si>
+    <t>Hadley Wickham</t>
+  </si>
+  <si>
+    <t>Garrett Grolemund</t>
+  </si>
+  <si>
+    <t>Charles Wheelan</t>
+  </si>
+  <si>
+    <t>Мертвые души</t>
+  </si>
+  <si>
+    <t>преступление и наказание</t>
+  </si>
+  <si>
+    <t>Идиот</t>
+  </si>
+  <si>
+    <t>Бесы</t>
+  </si>
+  <si>
+    <t>Братья Карамазовы</t>
+  </si>
+  <si>
+    <t>Война и мир</t>
+  </si>
+  <si>
+    <t>Анна Каренина</t>
+  </si>
+  <si>
+    <t>Смерть Ивана Ильича</t>
+  </si>
+  <si>
+    <t>Илиада</t>
+  </si>
+  <si>
+    <t>Одиссея</t>
+  </si>
+  <si>
+    <t>Моби Дик</t>
+  </si>
+  <si>
+    <t>Приключения Гекльберри Финна</t>
+  </si>
+  <si>
+    <t>Листья травы</t>
+  </si>
+  <si>
+    <t>Гамлет</t>
+  </si>
+  <si>
+    <t>Король Лир</t>
+  </si>
+  <si>
+    <t>Отелло</t>
+  </si>
+  <si>
+    <t>Тысяча и одна ночь</t>
+  </si>
+  <si>
+    <t>Грозовой перевал</t>
+  </si>
+  <si>
+    <t>Фауст</t>
+  </si>
+  <si>
+    <t>Божественная комедия</t>
+  </si>
+  <si>
+    <t>Отец Горио</t>
+  </si>
+  <si>
+    <t>Посторонний</t>
+  </si>
+  <si>
+    <t>Воспитание чувств</t>
+  </si>
+  <si>
+    <t>Старик и море</t>
+  </si>
+  <si>
+    <t>Альбер Камю</t>
+  </si>
+  <si>
+    <t>Антон Чехов</t>
+  </si>
+  <si>
+    <t>Вирджиния вулф</t>
+  </si>
+  <si>
+    <t>Гомер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гюстав Флобер </t>
+  </si>
+  <si>
+    <t>Дате Алигьери</t>
+  </si>
+  <si>
+    <t>Дени Дидро</t>
+  </si>
+  <si>
+    <t>Джакомо Леопарди</t>
+  </si>
+  <si>
+    <t>Джейн Остин</t>
+  </si>
+  <si>
+    <t>Джордж Оруэлл</t>
+  </si>
+  <si>
+    <t>Иоганн Вольфганг фон Гёте</t>
+  </si>
+  <si>
+    <t>Лев Толстой</t>
+  </si>
+  <si>
+    <t>Лу Синь</t>
+  </si>
+  <si>
+    <t>Марк Твен</t>
+  </si>
+  <si>
+    <t>Ральф Эллисон</t>
+  </si>
+  <si>
+    <t>Саади</t>
+  </si>
+  <si>
+    <t>Уильям Шекспир</t>
+  </si>
+  <si>
+    <t>Фёдор Достоевский</t>
+  </si>
+  <si>
+    <t>Эдгар Аллан По</t>
+  </si>
+  <si>
+    <t>The Pilgrim’s Progress</t>
+  </si>
+  <si>
+    <t>John Bunyan</t>
+  </si>
+  <si>
+    <t>Robinson Crusoe</t>
+  </si>
+  <si>
+    <t>Daniel Defoe</t>
+  </si>
+  <si>
+    <t> Jonathan Swift</t>
+  </si>
+  <si>
+    <t>Gulliver’s Travels</t>
+  </si>
+  <si>
+    <t>Samuel Richardson</t>
+  </si>
+  <si>
+    <t>Tom Jones</t>
+  </si>
+  <si>
+    <t>Henry Fielding </t>
+  </si>
+  <si>
+    <t>The Life and Opinions of Tristram Shandy</t>
+  </si>
+  <si>
+    <t>Clarissa</t>
+  </si>
+  <si>
+    <t>Gentleman</t>
+  </si>
+  <si>
+    <t>Laurence Sterne</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Jane Austen</t>
+  </si>
+  <si>
+    <t>Frankenstein</t>
+  </si>
+  <si>
+    <t>Mary Shelley</t>
+  </si>
+  <si>
+    <t>Nightmare Abbey</t>
+  </si>
+  <si>
+    <t>Thomas Love Peacock</t>
+  </si>
+  <si>
+    <t>The Narrative of Arthur Gordon Pym of Nantucket</t>
+  </si>
+  <si>
+    <t>Edgar Allan Poe</t>
+  </si>
+  <si>
+    <t>Sybil</t>
+  </si>
+  <si>
+    <t>Benjamin Disraeli</t>
+  </si>
+  <si>
+    <t>Jane Eyre</t>
+  </si>
+  <si>
+    <t>Charlotte Brontë</t>
+  </si>
+  <si>
+    <t>Wuthering Heights </t>
+  </si>
+  <si>
+    <t>Emily Brontë</t>
+  </si>
+  <si>
+    <t>Vanity Fair</t>
+  </si>
+  <si>
+    <t>William Thackeray</t>
+  </si>
+  <si>
+    <t>David Copperfield</t>
+  </si>
+  <si>
+    <t>Charles Dickens</t>
   </si>
 </sst>
 </file>
@@ -125,9 +489,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -519,4 +884,716 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD8FFB-76E5-42D6-97ED-BA63F04AA3CA}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1341487A-29B8-4B8C-B626-95580E8815B9}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0765593-42DD-42E8-965A-823CCFB79D3A}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE7FDD2-0457-4439-A107-EA4B1157F67D}">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.5546875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EDC7A9-A0E3-4A39-B407-3326ABC4D953}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D7FFE7-3841-40DC-8C08-DE9543B81FF8}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C1E4B8-2F38-4672-9364-D23A67111FBB}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>